<commit_message>
Validações do campo validade
</commit_message>
<xml_diff>
--- a/Produtos.xlsx
+++ b/Produtos.xlsx
@@ -2,28 +2,32 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4035" yWindow="2925" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,11 +50,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -122,6 +127,21 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TabelaProdutos" displayName="TabelaProdutos" ref="A1:F7" headerRowCount="1">
+  <autoFilter ref="A1:F2"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Nome do Produto"/>
+    <tableColumn id="2" name="Código de Barras"/>
+    <tableColumn id="3" name="Validade"/>
+    <tableColumn id="4" name="Fornecedor"/>
+    <tableColumn id="5" name="Categoria"/>
+    <tableColumn id="6" name="Observações"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,41 +433,44 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="6"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Nome do Produto</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Código de Barras</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Validade</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Fornecedor</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Categoria</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Observações</t>
         </is>
@@ -456,22 +479,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">arroz </t>
+          <t>Abacate Azedo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1234546</t>
+          <t>7102342899410</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01/08/2025</t>
+          <t>12/08/2005</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>cocal</t>
+          <t>Super 2</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -489,22 +512,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>arroz</t>
+          <t>Carne</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1234567894</t>
+          <t>038899421</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>05/05/2025</t>
+          <t>12/08/2005</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>cocal</t>
+          <t>Super 2</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -514,7 +537,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nenhuma observação
+          <t>
 </t>
         </is>
       </c>
@@ -522,22 +545,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>feijão</t>
+          <t>Carne</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>987654321</t>
+          <t>9402949421749</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>01/05/2025</t>
+          <t>12/08/2027</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>vasconlos</t>
+          <t>Super</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -547,12 +570,114 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve">nenhuma observação
+          <t>
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Carne ovina</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>49279941724</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>01/02/2027</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Super 2</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Alimento</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Ovo</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>749012421</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>12/03/2026</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Super 3</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Alimento</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ovos</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0281084014</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>12/08/2030</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Super 3</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Alimento</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>
 </t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
melhoria de (unidade) de produto
</commit_message>
<xml_diff>
--- a/Produtos.xlsx
+++ b/Produtos.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TabelaProdutos" displayName="TabelaProdutos" ref="A1:F5" headerRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TabelaProdutos" displayName="TabelaProdutos" ref="A1:G11" headerRowCount="1">
   <autoFilter ref="A1:F1"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Nome do Produto"/>
@@ -427,12 +427,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -612,10 +612,238 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Melão</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>super</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Alimento</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">boa
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Melão </t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>03/06/2025</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>super</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Alimento</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">é isso
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Melão</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>05/06/2025</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Super</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Alimento</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">é isso
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Melão</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>05/06/2025</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Super</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Alimento</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">É isso
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Melão</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>06/06/2025</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Super</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Alimento</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">É isso
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Melão</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>06/06/2025</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Super</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Alimento</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">É isso
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
pesquisa e edição, melhorias de estilo e tamanho
</commit_message>
<xml_diff>
--- a/Produtos.xlsx
+++ b/Produtos.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TabelaProdutos" displayName="TabelaProdutos" ref="A1:G11" headerRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TabelaProdutos" displayName="TabelaProdutos" ref="A1:G13" headerRowCount="1">
   <autoFilter ref="A1:F1"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Nome do Produto"/>
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -840,6 +840,82 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Maçã</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>001</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>17/05/2025</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>super</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Alimento</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Verde
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Melão</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>777</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>02/06/2025</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>super</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Alimento</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">

</xml_diff>